<commit_message>
Load rooming list v1
</commit_message>
<xml_diff>
--- a/app/templates/report/rooming.xlsx
+++ b/app/templates/report/rooming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ADFF1E-7592-4D1C-AFDC-D0357E7A96E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7EC31C-930D-468A-9D48-5BF025451B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>ROOMING LIST</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Booking_id</t>
   </si>
   <si>
-    <t>Resource_id</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>Nationality.Name</t>
   </si>
   <si>
-    <t>Origin.Name</t>
-  </si>
-  <si>
     <t>Tipo de documento</t>
   </si>
   <si>
@@ -157,6 +151,12 @@
   </si>
   <si>
     <t>País de origen</t>
+  </si>
+  <si>
+    <t>Country_origin.Name</t>
+  </si>
+  <si>
+    <t>Resource.Code</t>
   </si>
 </sst>
 </file>
@@ -1056,19 +1056,19 @@
         <v>4</v>
       </c>
       <c r="E3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>6</v>
@@ -1089,23 +1089,25 @@
         <v>11</v>
       </c>
       <c r="P3" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="R3" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="25" t="s">
+        <v>39</v>
+      </c>
       <c r="C4" s="24" t="s">
         <v>12</v>
       </c>
@@ -1116,7 +1118,7 @@
         <v>21</v>
       </c>
       <c r="F4" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="28" t="s">
         <v>14</v>
@@ -1125,7 +1127,7 @@
         <v>15</v>
       </c>
       <c r="I4" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J4" s="28" t="s">
         <v>6</v>
@@ -1146,16 +1148,16 @@
         <v>20</v>
       </c>
       <c r="P4" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="29" t="s">
-        <v>30</v>
-      </c>
       <c r="S4" s="25" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1213,13 +1215,13 @@
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>15</v>
@@ -1255,13 +1257,13 @@
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>15</v>
@@ -1297,13 +1299,13 @@
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>15</v>
@@ -1339,13 +1341,13 @@
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="33"/>
     </row>
     <row r="2" spans="1:2" s="10" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="25" t="s">
         <v>15</v>

</xml_diff>